<commit_message>
adding scapula trait terms
</commit_message>
<xml_diff>
--- a/terms/scapulaTerms.xlsx
+++ b/terms/scapulaTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meghanabalk/GitHub/futres/fovt/terms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD4E95-9ECB-7A4D-89EB-669351C67DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5239CD6A-E9C0-9744-B548-AEF2EEE1F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="620" windowWidth="14400" windowHeight="12660" activeTab="1" xr2:uid="{EA1FFA2F-09CB-F14C-A741-66F5F16569C3}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="8320" xr2:uid="{EA1FFA2F-09CB-F14C-A741-66F5F16569C3}"/>
   </bookViews>
   <sheets>
     <sheet name="trait" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>FOVT STATUS</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>neck of scapula</t>
+  </si>
+  <si>
+    <t>in oba</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>in fovt</t>
   </si>
 </sst>
 </file>
@@ -568,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C644AB-D3DB-D847-AAAF-F3E155F94507}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,6 +615,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
@@ -620,6 +632,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
       <c r="C4" t="s">
         <v>46</v>
       </c>
@@ -631,6 +649,12 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
       <c r="C5" t="s">
         <v>45</v>
       </c>
@@ -642,6 +666,12 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
@@ -673,6 +703,12 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
       <c r="C8" t="s">
         <v>43</v>
       </c>
@@ -687,6 +723,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
       <c r="C9" t="s">
         <v>44</v>
       </c>
@@ -701,6 +743,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
       <c r="C10" t="s">
         <v>42</v>
       </c>
@@ -725,6 +773,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -732,11 +781,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF42018-2D6B-7D49-894E-E8D531DB42FC}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -888,7 +940,7 @@
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>